<commit_message>
add project risks to register
</commit_message>
<xml_diff>
--- a/UI_Enterprise_Transformation/LO1.xlsx
+++ b/UI_Enterprise_Transformation/LO1.xlsx
@@ -17,9 +17,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
-  <si>
-    <t xml:space="preserve">Risk Tracking Template</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="89">
+  <si>
+    <t xml:space="preserve">Risk Tracking Template MAUIS</t>
   </si>
   <si>
     <t xml:space="preserve">Date of last review:</t>
@@ -208,7 +208,7 @@
     <t xml:space="preserve">Leads to fines and loss of customer confidence</t>
   </si>
   <si>
-    <t xml:space="preserve">Design with privacy in mind, follow GDPR practices</t>
+    <t xml:space="preserve">Design with privacy in mind, follow GDPR practices, Team Training</t>
   </si>
   <si>
     <t xml:space="preserve">Legal/Dev Team</t>
@@ -230,6 +230,30 @@
   </si>
   <si>
     <t xml:space="preserve">Review platform requirements for tracking data, build app consenting to these.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Key Team members sickness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Loss of team momentum </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Design documentation for development, clear goals defined and backlog of tasks arranged into sprints</t>
+  </si>
+  <si>
+    <t>Management</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scope Creep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Goals become diluted with new less necessary tasks, original scope gets pushed back.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clear design documentation, team keeps to Agile principles and Scrum master and Product Owner keep development focussed and a tight feedback loop with stakeholders.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scrum Master, ProductOwner</t>
   </si>
   <si>
     <t>Introduction</t>
@@ -1209,7 +1233,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="B3" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="B17" zoomScale="100" workbookViewId="0">
       <selection activeCell="D34" activeCellId="0" sqref="D34"/>
     </sheetView>
   </sheetViews>
@@ -1220,7 +1244,7 @@
     <col customWidth="1" min="4" max="4" width="12.8515625"/>
     <col customWidth="1" min="5" max="5" width="13.140625"/>
     <col customWidth="1" min="6" max="6" width="13.7109375"/>
-    <col customWidth="1" min="7" max="7" width="54.8515625"/>
+    <col customWidth="1" min="7" max="7" width="81.7109375"/>
     <col customWidth="1" min="8" max="8" width="17.44140625"/>
     <col customWidth="1" min="9" max="9" width="25.6640625"/>
   </cols>
@@ -1864,8 +1888,27 @@
       <c r="A22" s="12">
         <v>17</v>
       </c>
-      <c r="G22" s="20"/>
-      <c r="H22" s="12"/>
+      <c r="B22" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="G22" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="H22" s="12" t="s">
+        <v>74</v>
+      </c>
       <c r="I22" s="17"/>
       <c r="J22" s="18"/>
       <c r="K22" s="18"/>
@@ -1878,8 +1921,27 @@
       <c r="A23" s="12">
         <v>18</v>
       </c>
-      <c r="G23" s="20"/>
-      <c r="H23" s="12"/>
+      <c r="B23" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="F23" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="G23" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="H23" s="12" t="s">
+        <v>78</v>
+      </c>
       <c r="I23" s="17"/>
       <c r="J23" s="18"/>
       <c r="K23" s="18"/>
@@ -2119,52 +2181,52 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="29" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" ht="57.600000000000001">
       <c r="A3" s="30" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="31" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>